<commit_message>
Now has capibility to work for both PSX and QSE
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c77e18fefdda148/VSCODE/Python_PSX_Stock_Scanner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="13_ncr:1_{BDEFF61A-D09C-4321-9DC2-F0E62593C933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95596DEE-9481-47BD-BB8C-2F7D3EAB97AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A5AF3-971A-4DBE-9AC6-EF3522B0741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="271">
   <si>
     <t>MLCF</t>
   </si>
@@ -842,6 +842,18 @@
   </si>
   <si>
     <t>BEMA</t>
+  </si>
+  <si>
+    <t>KSE100</t>
+  </si>
+  <si>
+    <t>KSE30</t>
+  </si>
+  <si>
+    <t>ALLSHR</t>
+  </si>
+  <si>
+    <t>GNRI</t>
   </si>
 </sst>
 </file>
@@ -1901,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4494E4DA-CD44-41F0-A2A2-23143E103CC7}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="A31" sqref="A31:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,6 +2075,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A30">
     <sortCondition ref="A20:A30"/>
@@ -2074,10 +2101,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780D24C6-A9D5-46F4-98A9-E71F53C37CF2}">
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,6 +2430,21 @@
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2416,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3395A89D-3CD4-42FD-BD38-F624E537CB75}">
-  <dimension ref="A1:A211"/>
+  <dimension ref="A1:A214"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="A212" sqref="A212:A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3483,6 +3525,21 @@
         <v>139</v>
       </c>
     </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A211">
     <sortCondition ref="A174:A211"/>
@@ -3494,10 +3551,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE23DA-1E37-4AB0-A620-D635E6533091}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3765,6 +3822,11 @@
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3776,7 +3838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
no of shares will be printed in email message and strong buy condition will dipalyed on the emial message
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EDFC06-B54C-4702-865C-2150D67A4918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CC2D8D-0737-46BB-B7D9-CF7CBA6B5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="273">
   <si>
     <t>MLCF</t>
   </si>
@@ -1419,7 +1419,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1427,27 +1427,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00AA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00AA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00AA00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3884,10 +3863,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,19 +4047,29 @@
         <v>272</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A22" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="4" priority="3">
+  <conditionalFormatting sqref="A1:A22">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($J1&gt;50, $L1&gt;0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:A22">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>AND($J18&gt;50, $L18&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
PSX data reader with strategy tester
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CC2D8D-0737-46BB-B7D9-CF7CBA6B5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA55F2F6-C282-44B8-9A3C-A26F92A91F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="271">
   <si>
     <t>MLCF</t>
   </si>
@@ -631,16 +631,10 @@
     <t>BATA</t>
   </si>
   <si>
-    <t>MEEZ</t>
-  </si>
-  <si>
     <t>AGSML</t>
   </si>
   <si>
     <t>ASL</t>
-  </si>
-  <si>
-    <t>MLT</t>
   </si>
   <si>
     <t>WHALE</t>
@@ -1747,191 +1741,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847195A8-7734-4B43-8572-329A7797E7C5}">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A34">
-    <sortCondition ref="A20:A34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A32">
+    <sortCondition ref="A18:A32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1946,175 +1930,175 @@
       <selection activeCell="A31" sqref="A31:A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2134,344 +2118,344 @@
       <selection activeCell="A65" sqref="A65:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2491,1080 +2475,1080 @@
       <selection activeCell="A212" sqref="A212:A214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A160" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3584,276 +3568,276 @@
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3865,201 +3849,201 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed misc scripts folder
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA55F2F6-C282-44B8-9A3C-A26F92A91F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AF55B5-B348-484D-8BB0-82C2B6DAA79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="271">
   <si>
     <t>MLCF</t>
   </si>
@@ -1741,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847195A8-7734-4B43-8572-329A7797E7C5}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1913,6 +1913,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A32">
     <sortCondition ref="A18:A32"/>
@@ -1924,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4494E4DA-CD44-41F0-A2A2-23143E103CC7}">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2093,11 +2103,6 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2469,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3395A89D-3CD4-42FD-BD38-F624E537CB75}">
-  <dimension ref="A1:A214"/>
+  <dimension ref="A1:A213"/>
   <sheetViews>
     <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212:A214"/>
+      <selection activeCell="A213" sqref="A213:XFD213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3543,11 +3548,6 @@
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A214" s="1" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3850,7 +3850,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4035,15 +4035,24 @@
       <c r="A23" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="B23" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>267</v>
       </c>
+      <c r="B24" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>266</v>
+      </c>
+      <c r="B25" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update only no script change
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AF55B5-B348-484D-8BB0-82C2B6DAA79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25352971-99CB-4A54-9F1E-923C71A5C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="270">
   <si>
     <t>MLCF</t>
   </si>
@@ -845,9 +845,6 @@
   </si>
   <si>
     <t>KSE30</t>
-  </si>
-  <si>
-    <t>ALLSHR</t>
   </si>
   <si>
     <t>GNRI</t>
@@ -1936,7 +1933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4494E4DA-CD44-41F0-A2A2-23143E103CC7}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -2117,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780D24C6-A9D5-46F4-98A9-E71F53C37CF2}">
-  <dimension ref="A1:A67"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:A67"/>
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2455,11 +2452,6 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3837,7 +3829,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3847,10 +3839,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3860,7 +3852,7 @@
         <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -3868,7 +3860,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -3876,7 +3868,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -3884,7 +3876,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -3892,7 +3884,7 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -3900,7 +3892,7 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -3908,7 +3900,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -3916,7 +3908,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -3924,7 +3916,7 @@
         <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -3932,7 +3924,7 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3940,7 +3932,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3948,7 +3940,7 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -3956,7 +3948,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -3964,7 +3956,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3972,7 +3964,7 @@
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3980,7 +3972,7 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -3988,7 +3980,7 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -3996,7 +3988,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -4004,7 +3996,7 @@
         <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -4012,7 +4004,7 @@
         <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -4020,7 +4012,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -4028,7 +4020,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -4036,23 +4028,15 @@
         <v>265</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duplicate psx folder deleted
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25352971-99CB-4A54-9F1E-923C71A5C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF94DB84-9A6E-476C-9DDF-08ADFD6F953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="266">
   <si>
     <t>MLCF</t>
   </si>
@@ -700,9 +700,6 @@
     <t>MARK</t>
   </si>
   <si>
-    <t>CBQK</t>
-  </si>
-  <si>
     <t>DUBK</t>
   </si>
   <si>
@@ -727,9 +724,6 @@
     <t>BRES</t>
   </si>
   <si>
-    <t>ABQK</t>
-  </si>
-  <si>
     <t>QATI</t>
   </si>
   <si>
@@ -790,9 +784,6 @@
     <t>QISI</t>
   </si>
   <si>
-    <t>DOHI</t>
-  </si>
-  <si>
     <t>QGRI</t>
   </si>
   <si>
@@ -836,9 +827,6 @@
   </si>
   <si>
     <t>QGMD</t>
-  </si>
-  <si>
-    <t>BEMA</t>
   </si>
   <si>
     <t>KSE100</t>
@@ -1912,12 +1900,12 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2095,12 +2083,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2447,12 +2435,12 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3535,12 +3523,12 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3554,10 +3542,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE23DA-1E37-4AB0-A620-D635E6533091}">
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3809,27 +3797,7 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3841,7 +3809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
@@ -3852,7 +3820,7 @@
         <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -3860,7 +3828,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -3868,7 +3836,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -3876,7 +3844,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -3884,7 +3852,7 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -3892,7 +3860,7 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -3900,7 +3868,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -3908,7 +3876,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -3916,7 +3884,7 @@
         <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -3924,7 +3892,7 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3932,7 +3900,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3940,7 +3908,7 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -3948,7 +3916,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -3956,7 +3924,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3964,7 +3932,7 @@
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3972,7 +3940,7 @@
         <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -3980,7 +3948,7 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -3988,7 +3956,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -3996,7 +3964,7 @@
         <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -4004,7 +3972,7 @@
         <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -4012,7 +3980,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -4020,23 +3988,23 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B23" t="s">
         <v>265</v>
-      </c>
-      <c r="B23" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest commit form te aws server 1 till today 16 march 2024
</commit_message>
<xml_diff>
--- a/PSXSymbols.xlsx
+++ b/PSXSymbols.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\Python_PSX_Stock_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF94DB84-9A6E-476C-9DDF-08ADFD6F953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72515FE-6C89-4F99-812F-E53761E33227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11265" activeTab="3" xr2:uid="{3F91CB41-9821-4D9A-973E-13C63C7D8708}"/>
   </bookViews>
   <sheets>
     <sheet name="MYLIST" sheetId="4" r:id="rId1"/>
     <sheet name="KMI30" sheetId="3" r:id="rId2"/>
     <sheet name="KMI100" sheetId="2" r:id="rId3"/>
-    <sheet name="KMIALL" sheetId="1" r:id="rId4"/>
-    <sheet name="QSE" sheetId="5" r:id="rId5"/>
-    <sheet name="CUSTUM" sheetId="6" r:id="rId6"/>
+    <sheet name="CRYPTO" sheetId="7" r:id="rId4"/>
+    <sheet name="KMIALL" sheetId="1" r:id="rId5"/>
+    <sheet name="QSE" sheetId="5" r:id="rId6"/>
+    <sheet name="CUSTUM" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CUSTUM!$A$1:$A$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CUSTUM!$A$1:$A$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="321">
   <si>
     <t>MLCF</t>
   </si>
@@ -842,13 +843,178 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>PTCA</t>
+  </si>
+  <si>
+    <t>MYLIST</t>
+  </si>
+  <si>
+    <t>RMPL</t>
+  </si>
+  <si>
+    <t>NESTLE</t>
+  </si>
+  <si>
+    <t>MZNPETF</t>
+  </si>
+  <si>
+    <t>BTCUSDT</t>
+  </si>
+  <si>
+    <t>ETHUSDT</t>
+  </si>
+  <si>
+    <t>BNBUSDT</t>
+  </si>
+  <si>
+    <t>XRPUSDT</t>
+  </si>
+  <si>
+    <t>ADAUSDT</t>
+  </si>
+  <si>
+    <t>SOLUSDT</t>
+  </si>
+  <si>
+    <t>DOGEUSDT</t>
+  </si>
+  <si>
+    <t>DOTUSDT</t>
+  </si>
+  <si>
+    <t>LINKUSDT</t>
+  </si>
+  <si>
+    <t>LTCUSDT</t>
+  </si>
+  <si>
+    <t>BCHUSDT</t>
+  </si>
+  <si>
+    <t>MATICUSDT</t>
+  </si>
+  <si>
+    <t>ETCUSDT</t>
+  </si>
+  <si>
+    <t>VETUSDT</t>
+  </si>
+  <si>
+    <t>FILUSDT</t>
+  </si>
+  <si>
+    <t>UNIUSDT</t>
+  </si>
+  <si>
+    <t>TRXUSDT</t>
+  </si>
+  <si>
+    <t>XLMUSDT</t>
+  </si>
+  <si>
+    <t>ICPUSDT</t>
+  </si>
+  <si>
+    <t>EOSUSDT</t>
+  </si>
+  <si>
+    <t>ATOMUSDT</t>
+  </si>
+  <si>
+    <t>XTZUSDT</t>
+  </si>
+  <si>
+    <t>XMRUSDT</t>
+  </si>
+  <si>
+    <t>CAKEUSDT</t>
+  </si>
+  <si>
+    <t>ALGOUSDT</t>
+  </si>
+  <si>
+    <t>WAVESUSDT</t>
+  </si>
+  <si>
+    <t>AAVEUSDT</t>
+  </si>
+  <si>
+    <t>FTTUSDT</t>
+  </si>
+  <si>
+    <t>DASHUSDT</t>
+  </si>
+  <si>
+    <t>IOTAUSDT</t>
+  </si>
+  <si>
+    <t>MKRUSDT</t>
+  </si>
+  <si>
+    <t>SHIBUSDT</t>
+  </si>
+  <si>
+    <t>NEARUSDT</t>
+  </si>
+  <si>
+    <t>MANAUSDT</t>
+  </si>
+  <si>
+    <t>GRTUSDT</t>
+  </si>
+  <si>
+    <t>ENJUSDT</t>
+  </si>
+  <si>
+    <t>ZECUSDT</t>
+  </si>
+  <si>
+    <t>SUSHIUSDT</t>
+  </si>
+  <si>
+    <t>COMPUSDT</t>
+  </si>
+  <si>
+    <t>QTUMUSDT</t>
+  </si>
+  <si>
+    <t>SNXUSDT</t>
+  </si>
+  <si>
+    <t>YFIUSDT</t>
+  </si>
+  <si>
+    <t>RVNUSDT</t>
+  </si>
+  <si>
+    <t>EGLDUSDT</t>
+  </si>
+  <si>
+    <t>CRVUSDT</t>
+  </si>
+  <si>
+    <t>KSMUSDT</t>
+  </si>
+  <si>
+    <t>ZILUSDT</t>
+  </si>
+  <si>
+    <t>RUNEUSDT</t>
+  </si>
+  <si>
+    <t>LUNAUSDT</t>
+  </si>
+  <si>
+    <t>STMXUSDT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,8 +1149,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF363636"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1162,6 +1340,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1349,10 +1533,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1430,9 +1620,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1470,7 +1660,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1576,7 +1766,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1718,7 +1908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1728,182 +1918,182 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847195A8-7734-4B43-8572-329A7797E7C5}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>262</v>
       </c>
@@ -1925,168 +2115,168 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>262</v>
       </c>
@@ -2102,350 +2292,562 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780D24C6-A9D5-46F4-98A9-E71F53C37CF2}">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A73" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="12" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B14" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B21" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B34" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B38" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B47" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="B50" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="B51" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="B52" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="B53" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B57" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="B58" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="B59" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="B60" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="B61" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="B62" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="B63" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="B67" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="B75" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="B80" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>262</v>
+      <c r="B83" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A64">
-    <sortCondition ref="A1:A64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B86">
+    <sortCondition ref="A73:A86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2453,6 +2855,274 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA19FD0-C43B-4083-9CCE-9A78B6A675E9}">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3395A89D-3CD4-42FD-BD38-F624E537CB75}">
   <dimension ref="A1:A213"/>
   <sheetViews>
@@ -2460,1073 +3130,1073 @@
       <selection activeCell="A213" sqref="A213:XFD213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>262</v>
       </c>
@@ -3540,262 +4210,262 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE23DA-1E37-4AB0-A620-D635E6533091}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>263</v>
       </c>
@@ -3805,7 +4475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ED9EAE-1B43-47FE-9FEF-A9FEA7FC572F}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -3813,9 +4483,9 @@
       <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -3823,7 +4493,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3831,7 +4501,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -3839,7 +4509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3847,7 +4517,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3855,7 +4525,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -3863,7 +4533,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3871,7 +4541,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -3879,7 +4549,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -3887,7 +4557,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3895,7 +4565,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3903,7 +4573,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3911,7 +4581,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -3919,7 +4589,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3927,7 +4597,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -3935,7 +4605,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -3943,7 +4613,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -3951,7 +4621,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -3959,7 +4629,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3967,7 +4637,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3975,7 +4645,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3983,7 +4653,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3991,7 +4661,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>261</v>
       </c>
@@ -3999,7 +4669,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>262</v>
       </c>

</xml_diff>